<commit_message>
update report sprint 3
</commit_message>
<xml_diff>
--- a/Report/Sprint_review.xlsx
+++ b/Report/Sprint_review.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Spring 1" sheetId="1" r:id="rId1"/>
     <sheet name="Spring 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Spring 3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="40">
   <si>
     <t>MSSV</t>
   </si>
@@ -92,6 +93,60 @@
   </si>
   <si>
     <t>Sprint 2</t>
+  </si>
+  <si>
+    <t>Xử lý giao diện profile
+Xử lý code behind cho màn hình đặt thuyền để vào game</t>
+  </si>
+  <si>
+    <t>80%
+100%</t>
+  </si>
+  <si>
+    <t>Thiết kế giao diện profile và các item
+Thiết kế giao diện cho thuyền và background
+Tìm kiếm và thiết lập kết nối giữa hai thiết bị qua bluetooth</t>
+  </si>
+  <si>
+    <t>50%
+50%
+80%</t>
+  </si>
+  <si>
+    <t>Xây dựng UI cho màn hình đặt thuyền</t>
+  </si>
+  <si>
+    <t>Tổng kết trong tuần vừa qua bọn em gặp phải một số vấn đề như sau:</t>
+  </si>
+  <si>
+    <t>Do design bọn e tự thiết kế nên một số màn hình như màn hình đặt thuyền trước khi vào game hay phần profile chỗ skin/background vẫn chờ hình vẽ xong</t>
+  </si>
+  <si>
+    <t>Kết nối giữa hai thiết bị qua bluetooth đã làm được nhưng vẫn còn mắc nhiều lỗi do sự khác nhau giữa các phiên bản Android</t>
+  </si>
+  <si>
+    <t>Do có nhiều thread chạy ngầm nên có 1 điện thoại đã không demo được vì gặp phải vấn đề memory lead.</t>
+  </si>
+  <si>
+    <t>Một số thành viên đến bây giờ vẫn không có đóng góp gì cho nhóm, bọn e vẫn đang cân nhắc xem đến kết thúc project bạn ấy có đóng góp gì không, việc này em sẽ thông báo cho thầy sau nha thầy.</t>
+  </si>
+  <si>
+    <t>Sprint 3</t>
+  </si>
+  <si>
+    <t>Màn hình item trong Profile</t>
+  </si>
+  <si>
+    <t>Màn hình lịch sử đấu</t>
+  </si>
+  <si>
+    <t>Màn hình hostgame</t>
+  </si>
+  <si>
+    <t>Màn hình join game</t>
+  </si>
+  <si>
+    <t>Màn hình đặt thuyền trước khi vào game</t>
   </si>
 </sst>
 </file>
@@ -178,7 +233,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -187,6 +242,28 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -282,6 +359,231 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1717030</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="4533900"/>
+          <a:ext cx="4641205" cy="10058400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1717030</xdr:colOff>
+      <xdr:row>131</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="15582900"/>
+          <a:ext cx="4641205" cy="10058400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>135</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1717030</xdr:colOff>
+      <xdr:row>187</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="26250900"/>
+          <a:ext cx="4641205" cy="10058400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>194</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1717030</xdr:colOff>
+      <xdr:row>246</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="37490400"/>
+          <a:ext cx="4641205" cy="10058400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>251</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1717030</xdr:colOff>
+      <xdr:row>303</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="48348900"/>
+          <a:ext cx="4641205" cy="10058400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -688,8 +990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -813,4 +1115,180 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:F250"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A244" workbookViewId="0">
+      <selection activeCell="D249" sqref="D249"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="3" max="3" width="24" customWidth="1"/>
+    <col min="4" max="4" width="61.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" customWidth="1"/>
+    <col min="6" max="6" width="46.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="6">
+        <v>1412180</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="6"/>
+    </row>
+    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B5" s="6">
+        <v>1412168</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="6"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="6">
+        <v>1412175</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="6">
+        <v>1512051</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="6">
+        <v>1712414</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="8">
+        <v>1</v>
+      </c>
+      <c r="F8" s="6"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B78" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="134" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B134" s="13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="193" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B193" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="250" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B250" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Implement display location which has been shot
</commit_message>
<xml_diff>
--- a/Report/Sprint_review.xlsx
+++ b/Report/Sprint_review.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1" sheetId="1" r:id="rId1"/>
     <sheet name="Sprint 2" sheetId="2" r:id="rId2"/>
     <sheet name="Sprint 3" sheetId="3" r:id="rId3"/>
     <sheet name="Sprint 4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sprint 5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="65">
   <si>
     <t>MSSV</t>
   </si>
@@ -196,6 +197,48 @@
   </si>
   <si>
     <t>Màn hình sau khi đã cài thuyền xong cả 2 bắt đầu trận chiến</t>
+  </si>
+  <si>
+    <t>Xử lý logic giữa các lượt bắn cũng như việc gửi các lệnh bắn qua lại giữa 2 điện thoại
+Fix bug consitence về thời gian đếm ngược khi vào màn hình bắt đầu của 2 điện thoại</t>
+  </si>
+  <si>
+    <t>80%
+80%
+100%
+100%</t>
+  </si>
+  <si>
+    <t>Qui định các gói tin qua lại giữa 2 điện thoại</t>
+  </si>
+  <si>
+    <t>100%
+30%
+80%</t>
+  </si>
+  <si>
+    <t>test màn hình game play</t>
+  </si>
+  <si>
+    <t>Fix bug màn hình gameplay</t>
+  </si>
+  <si>
+    <t>Sprint 5</t>
+  </si>
+  <si>
+    <t>Các bug về kết nối bluetooth như là ngắt kết nối giữa chừng vẫn chưa xử lý được</t>
+  </si>
+  <si>
+    <t>Nhiều thành viên vẫn còn khá bận để dành thời gian cho việc kết thúc đồ án</t>
+  </si>
+  <si>
+    <t>Phần giao diện bị đứng hẳn do tuần rồi bạn làm giao diện cũng khá bận nhiều công việc nên việc background căng không chuẩn với các ô của grid hay kí hiệu khi bị bắn còn hơi xấu, em chỉ đang để tạm sau này có design rồi bọn e sẽ sửa sau ạ</t>
+  </si>
+  <si>
+    <t>Màn hình map của mình sau 4 lượt bắn. Tất cả viên đạn mà địch bắn được đánh bằng dấu X trên map, bắn rồi sẽ không bắn được lại vào ô đó nữa.</t>
+  </si>
+  <si>
+    <t>Màn hình bên địch sau 4 lượt bắn của chúng ta, cả 4 lượt bắn đều trúng đích, một chiếc thuyền sau khi bị phá hủy hoàn toàn sẽ bị hiển thị trên map</t>
   </si>
 </sst>
 </file>
@@ -282,7 +325,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -313,6 +356,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -729,6 +775,99 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>3743325</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1304925" y="3238500"/>
+          <a:ext cx="5143500" cy="9144000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>3743325</xdr:colOff>
+      <xdr:row>115</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1304925" y="12954000"/>
+          <a:ext cx="5143500" cy="9144000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1439,8 +1578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B73" sqref="B73"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1588,4 +1727,153 @@
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:F67"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B67" sqref="B67"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="3" max="3" width="21" customWidth="1"/>
+    <col min="4" max="4" width="76" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="14">
+        <v>1412180</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" s="6"/>
+    </row>
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="6">
+        <v>1412168</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" s="6"/>
+    </row>
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="6">
+        <v>1412175</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" s="8">
+        <v>1</v>
+      </c>
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="6">
+        <v>1512051</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="12"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="6">
+        <v>1712414</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="8">
+        <v>1</v>
+      </c>
+      <c r="F8" s="6"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>